<commit_message>
Cap nhật Tim kiếm đơn hàng
</commit_message>
<xml_diff>
--- a/public/excel/baocao.xlsx
+++ b/public/excel/baocao.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="73">
   <si>
     <t>PHIẾU ĐỀ XUẤT HÀNG HÓA CĂN TIN</t>
   </si>
@@ -26,7 +26,7 @@
     <t>BỆNH VIỆN NHÂN ÁI</t>
   </si>
   <si>
-    <t>Từ ngày: 01-08-2022 đến ngày: 30-09-2022</t>
+    <t>Từ ngày: 01-08-2022 đến ngày: 30-10-2022</t>
   </si>
   <si>
     <t>STT</t>
@@ -173,19 +173,52 @@
     <t>A213</t>
   </si>
   <si>
+    <t>Cad điện thoại</t>
+  </si>
+  <si>
+    <t>TSDTK</t>
+  </si>
+  <si>
+    <t>B001</t>
+  </si>
+  <si>
+    <t>B004</t>
+  </si>
+  <si>
+    <t>40,000</t>
+  </si>
+  <si>
+    <t>B008</t>
+  </si>
+  <si>
+    <t>80,000</t>
+  </si>
+  <si>
+    <t>Nước yến</t>
+  </si>
+  <si>
+    <t>DK</t>
+  </si>
+  <si>
+    <t>Lon</t>
+  </si>
+  <si>
+    <t>CT5Z</t>
+  </si>
+  <si>
     <t>Tổng tiền</t>
   </si>
   <si>
-    <t>505,500</t>
+    <t>726,500</t>
   </si>
   <si>
     <t>Số tiền viết bằng chữ:</t>
   </si>
   <si>
-    <t>năm trăm  năm nghìn năm trăm đồng</t>
-  </si>
-  <si>
-    <t>ngày 09 tháng 09 năm 2022</t>
+    <t>bảy trăm  hai mươi sáu nghìn năm trăm đồng</t>
+  </si>
+  <si>
+    <t>ngày 03 tháng 10 năm 2022</t>
   </si>
   <si>
     <t>Người lập</t>
@@ -583,16 +616,16 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:I29"/>
+  <dimension ref="A1:I34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="I21" sqref="I21"/>
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="3" max="3" width="10" bestFit="true" customWidth="true" style="0"/>
-    <col min="2" max="2" width="39" bestFit="true" customWidth="true" style="0"/>
+    <col min="2" max="2" width="50" bestFit="true" customWidth="true" style="0"/>
     <col min="4" max="4" width="12" bestFit="true" customWidth="true" style="0"/>
     <col min="5" max="5" width="13" bestFit="true" customWidth="true" style="0"/>
     <col min="6" max="6" width="9" bestFit="true" customWidth="true" style="0"/>
@@ -1099,75 +1132,210 @@
       <c r="I21" s="5"/>
     </row>
     <row r="22" spans="1:9">
-      <c r="A22" t="s">
+      <c r="A22" s="5">
+        <v>17</v>
+      </c>
+      <c r="B22" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="B22"/>
-      <c r="C22"/>
-      <c r="D22"/>
-      <c r="E22"/>
-      <c r="F22"/>
-      <c r="G22"/>
-      <c r="H22" t="s">
+      <c r="C22" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="I22"/>
+      <c r="D22" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="G22" s="5">
+        <v>1</v>
+      </c>
+      <c r="H22" s="5">
+        <v>10000</v>
+      </c>
+      <c r="I22" s="5"/>
     </row>
     <row r="23" spans="1:9">
-      <c r="A23" t="s">
-        <v>54</v>
-      </c>
-      <c r="B23" t="s">
+      <c r="A23" s="5">
+        <v>18</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E23" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C23"/>
-      <c r="D23"/>
-      <c r="E23"/>
-      <c r="F23"/>
-      <c r="G23"/>
-      <c r="H23"/>
+      <c r="F23" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="G23" s="5">
+        <v>1</v>
+      </c>
+      <c r="H23" s="5">
+        <v>40000</v>
+      </c>
+      <c r="I23" s="5"/>
     </row>
     <row r="24" spans="1:9">
-      <c r="A24"/>
-      <c r="B24"/>
-      <c r="C24"/>
-      <c r="D24"/>
-      <c r="E24"/>
-      <c r="F24"/>
-      <c r="G24" t="s">
-        <v>56</v>
-      </c>
-      <c r="H24"/>
+      <c r="A24" s="5">
+        <v>19</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="G24" s="5">
+        <v>1</v>
+      </c>
+      <c r="H24" s="5">
+        <v>80000</v>
+      </c>
+      <c r="I24" s="5"/>
     </row>
     <row r="25" spans="1:9">
-      <c r="A25"/>
-      <c r="B25" t="s">
+      <c r="A25" s="5">
+        <v>20</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E25" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C25"/>
-      <c r="D25" t="s">
+      <c r="F25" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="E25"/>
-      <c r="F25"/>
-      <c r="G25" t="s">
+      <c r="G25" s="5">
+        <v>1</v>
+      </c>
+      <c r="H25" s="5">
+        <v>80000</v>
+      </c>
+      <c r="I25" s="5"/>
+    </row>
+    <row r="26" spans="1:9">
+      <c r="A26" s="5">
+        <v>21</v>
+      </c>
+      <c r="B26" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="H25"/>
+      <c r="C26" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G26" s="5">
+        <v>1</v>
+      </c>
+      <c r="H26" s="5">
+        <v>11000</v>
+      </c>
+      <c r="I26" s="5"/>
+    </row>
+    <row r="27" spans="1:9">
+      <c r="A27" t="s">
+        <v>63</v>
+      </c>
+      <c r="B27"/>
+      <c r="C27"/>
+      <c r="D27"/>
+      <c r="E27"/>
+      <c r="F27"/>
+      <c r="G27"/>
+      <c r="H27" t="s">
+        <v>64</v>
+      </c>
+      <c r="I27"/>
+    </row>
+    <row r="28" spans="1:9">
+      <c r="A28" t="s">
+        <v>65</v>
+      </c>
+      <c r="B28" t="s">
+        <v>66</v>
+      </c>
+      <c r="C28"/>
+      <c r="D28"/>
+      <c r="E28"/>
+      <c r="F28"/>
+      <c r="G28"/>
+      <c r="H28"/>
     </row>
     <row r="29" spans="1:9">
       <c r="A29"/>
-      <c r="B29" t="s">
-        <v>60</v>
-      </c>
+      <c r="B29"/>
       <c r="C29"/>
       <c r="D29"/>
       <c r="E29"/>
       <c r="F29"/>
       <c r="G29" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="H29"/>
+    </row>
+    <row r="30" spans="1:9">
+      <c r="A30"/>
+      <c r="B30" t="s">
+        <v>68</v>
+      </c>
+      <c r="C30"/>
+      <c r="D30" t="s">
+        <v>69</v>
+      </c>
+      <c r="E30"/>
+      <c r="F30"/>
+      <c r="G30" t="s">
+        <v>70</v>
+      </c>
+      <c r="H30"/>
+    </row>
+    <row r="34" spans="1:9">
+      <c r="A34"/>
+      <c r="B34" t="s">
+        <v>71</v>
+      </c>
+      <c r="C34"/>
+      <c r="D34"/>
+      <c r="E34"/>
+      <c r="F34"/>
+      <c r="G34" t="s">
+        <v>72</v>
+      </c>
+      <c r="H34"/>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>

</xml_diff>

<commit_message>
Cap Nhat thống kê
</commit_message>
<xml_diff>
--- a/public/excel/baocao.xlsx
+++ b/public/excel/baocao.xlsx
@@ -15,9 +15,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="25">
-  <si>
-    <t>PHIẾU ĐỀ XUẤT HÀNG HÓA CĂN TIN</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="76">
+  <si>
+    <t>BẢNG KÊ BÁN HÀNG CĂN TIN</t>
   </si>
   <si>
     <t>SỞ Y TẾ THÀNH PHỐ HỒ CHÍ MINH</t>
@@ -26,7 +26,7 @@
     <t>BỆNH VIỆN NHÂN ÁI</t>
   </si>
   <si>
-    <t>Từ ngày: 01-09-2022 đến ngày: 30-11-2022</t>
+    <t>Từ ngày: 01-08-2022 đến ngày: 02-11-2022</t>
   </si>
   <si>
     <t>STT</t>
@@ -38,6 +38,9 @@
     <t>Danh mục</t>
   </si>
   <si>
+    <t>Khoa</t>
+  </si>
+  <si>
     <t>ĐVT</t>
   </si>
   <si>
@@ -56,40 +59,190 @@
     <t>Ghi Chú</t>
   </si>
   <si>
+    <t>Bạc hà</t>
+  </si>
+  <si>
+    <t>TPCB</t>
+  </si>
+  <si>
+    <t>KN001</t>
+  </si>
+  <si>
+    <t>kg</t>
+  </si>
+  <si>
+    <t>A001</t>
+  </si>
+  <si>
+    <t>19,000</t>
+  </si>
+  <si>
+    <t>Bánh bèo</t>
+  </si>
+  <si>
+    <t>KN002</t>
+  </si>
+  <si>
+    <t>hộp</t>
+  </si>
+  <si>
+    <t>A002</t>
+  </si>
+  <si>
+    <t>17,000</t>
+  </si>
+  <si>
+    <t>Bột lộc</t>
+  </si>
+  <si>
+    <t>A003</t>
+  </si>
+  <si>
+    <t>Bánh bông lan</t>
+  </si>
+  <si>
+    <t>cái</t>
+  </si>
+  <si>
+    <t>A005</t>
+  </si>
+  <si>
+    <t>11,000</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>Bánh cam</t>
+  </si>
+  <si>
+    <t>A006</t>
+  </si>
+  <si>
+    <t>3,500</t>
+  </si>
+  <si>
+    <t>Bánh cưốn chả</t>
+  </si>
+  <si>
+    <t>A008</t>
+  </si>
+  <si>
+    <t>Bánh chưng nhỏ</t>
+  </si>
+  <si>
+    <t>cây</t>
+  </si>
+  <si>
+    <t>A009</t>
+  </si>
+  <si>
+    <t>Bánh cuốn</t>
+  </si>
+  <si>
+    <t>0,5kg</t>
+  </si>
+  <si>
+    <t>A192</t>
+  </si>
+  <si>
+    <t>10,000</t>
+  </si>
+  <si>
+    <t>Bánh ướt</t>
+  </si>
+  <si>
+    <t>A193</t>
+  </si>
+  <si>
+    <t>Bắp cải</t>
+  </si>
+  <si>
+    <t>A194</t>
+  </si>
+  <si>
+    <t>16,000</t>
+  </si>
+  <si>
     <t>Bột năng</t>
   </si>
   <si>
-    <t>TPCB</t>
-  </si>
-  <si>
     <t>0,1kg</t>
   </si>
   <si>
     <t>A200</t>
   </si>
   <si>
-    <t>3,500</t>
+    <t>Cà chua</t>
+  </si>
+  <si>
+    <t>A204</t>
+  </si>
+  <si>
+    <t>Cà pháo</t>
+  </si>
+  <si>
+    <t>A205</t>
+  </si>
+  <si>
+    <t>14,000</t>
+  </si>
+  <si>
+    <t>Cải thìa</t>
+  </si>
+  <si>
+    <t>A213</t>
+  </si>
+  <si>
+    <t>Cad điện thoại</t>
+  </si>
+  <si>
+    <t>TSDTK</t>
+  </si>
+  <si>
+    <t>B001</t>
+  </si>
+  <si>
+    <t>B004</t>
+  </si>
+  <si>
+    <t>40,000</t>
+  </si>
+  <si>
+    <t>B008</t>
+  </si>
+  <si>
+    <t>80,000</t>
   </si>
   <si>
     <t>Tổng tiền</t>
   </si>
   <si>
+    <t>719,000</t>
+  </si>
+  <si>
     <t>Số tiền viết bằng chữ:</t>
   </si>
   <si>
-    <t>ba nghìn năm trăm đồng</t>
-  </si>
-  <si>
-    <t>ngày 01 tháng 11 năm 2022</t>
-  </si>
-  <si>
-    <t>Giám đốc</t>
+    <t>bảy trăm  mười chín nghìn đồng</t>
+  </si>
+  <si>
+    <t>Ngày 02 tháng 11 năm 2022</t>
+  </si>
+  <si>
+    <t>Người lập</t>
   </si>
   <si>
     <t>PT Bộ Phận</t>
   </si>
   <si>
-    <t>Người đề nghị</t>
+    <t>kế toán</t>
+  </si>
+  <si>
+    <t>Lê Thị Hồng</t>
+  </si>
+  <si>
+    <t>Hoàng Thị Huệ</t>
   </si>
 </sst>
 </file>
@@ -472,36 +625,36 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:J34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="3" max="3" width="10" bestFit="true" customWidth="true" style="0"/>
-    <col min="2" max="2" width="26" bestFit="true" customWidth="true" style="0"/>
+    <col min="2" max="2" width="36" bestFit="true" customWidth="true" style="0"/>
     <col min="4" max="4" width="12" bestFit="true" customWidth="true" style="0"/>
-    <col min="5" max="5" width="13" bestFit="true" customWidth="true" style="0"/>
-    <col min="6" max="6" width="9" bestFit="true" customWidth="true" style="0"/>
+    <col min="5" max="5" width="6" bestFit="true" customWidth="true" style="0"/>
+    <col min="6" max="6" width="13" bestFit="true" customWidth="true" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:10">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:10">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
@@ -514,7 +667,7 @@
       <c r="H3" s="3"/>
       <c r="I3" s="2"/>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:10">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -526,7 +679,7 @@
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:10">
       <c r="A5" s="4" t="s">
         <v>4</v>
       </c>
@@ -554,100 +707,707 @@
       <c r="I5" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" spans="1:9">
+      <c r="J5" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
       <c r="A6" s="5">
         <v>1</v>
       </c>
       <c r="B6" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="H6" s="5">
+        <v>2</v>
+      </c>
+      <c r="I6" s="5">
+        <v>38000</v>
+      </c>
+      <c r="J6" s="5"/>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="5">
+        <v>2</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="H7" s="5">
+        <v>2</v>
+      </c>
+      <c r="I7" s="5">
+        <v>34000</v>
+      </c>
+      <c r="J7" s="5"/>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" s="5">
+        <v>3</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="5">
+        <v>1</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="H8" s="5">
+        <v>7</v>
+      </c>
+      <c r="I8" s="5">
+        <v>119000</v>
+      </c>
+      <c r="J8" s="5"/>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" s="5">
+        <v>4</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="5">
+        <v>1</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H9" s="5">
+        <v>8</v>
+      </c>
+      <c r="I9" s="5">
+        <v>88000</v>
+      </c>
+      <c r="J9" s="5"/>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" s="5">
+        <v>5</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H10" s="5">
+        <v>3</v>
+      </c>
+      <c r="I10" s="5">
+        <v>33000</v>
+      </c>
+      <c r="J10" s="5"/>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" s="5">
+        <v>6</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H11" s="5">
+        <v>1</v>
+      </c>
+      <c r="I11" s="5">
+        <v>11000</v>
+      </c>
+      <c r="J11" s="5"/>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12" s="5">
+        <v>7</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="H12" s="5">
+        <v>3</v>
+      </c>
+      <c r="I12" s="5">
+        <v>10500</v>
+      </c>
+      <c r="J12" s="5"/>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13" s="5">
+        <v>8</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="H13" s="5">
+        <v>1</v>
+      </c>
+      <c r="I13" s="5">
+        <v>17000</v>
+      </c>
+      <c r="J13" s="5"/>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14" s="5">
+        <v>9</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H14" s="5">
+        <v>1</v>
+      </c>
+      <c r="I14" s="5">
+        <v>11000</v>
+      </c>
+      <c r="J14" s="5"/>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="A15" s="5">
+        <v>10</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" s="5">
+        <v>1</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="H15" s="5">
+        <v>2</v>
+      </c>
+      <c r="I15" s="5">
+        <v>20000</v>
+      </c>
+      <c r="J15" s="5"/>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="A16" s="5">
+        <v>11</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" s="5">
+        <v>1</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="H16" s="5">
+        <v>2</v>
+      </c>
+      <c r="I16" s="5">
+        <v>20000</v>
+      </c>
+      <c r="J16" s="5"/>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17" s="5">
+        <v>12</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="H17" s="5">
+        <v>1</v>
+      </c>
+      <c r="I17" s="5">
+        <v>10000</v>
+      </c>
+      <c r="J17" s="5"/>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18" s="5">
         <v>13</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="B18" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D18" s="5">
+        <v>1</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="H18" s="5">
+        <v>2</v>
+      </c>
+      <c r="I18" s="5">
+        <v>32000</v>
+      </c>
+      <c r="J18" s="5"/>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19" s="5">
         <v>14</v>
       </c>
-      <c r="D6" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E6" s="5" t="s">
+      <c r="B19" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="H19" s="5">
+        <v>1</v>
+      </c>
+      <c r="I19" s="5">
+        <v>3500</v>
+      </c>
+      <c r="J19" s="5"/>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20" s="5">
+        <v>15</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="H20" s="5">
+        <v>2</v>
+      </c>
+      <c r="I20" s="5">
+        <v>34000</v>
+      </c>
+      <c r="J20" s="5"/>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="A21" s="5">
         <v>16</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="B21" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="G21" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="H21" s="5">
+        <v>1</v>
+      </c>
+      <c r="I21" s="5">
+        <v>14000</v>
+      </c>
+      <c r="J21" s="5"/>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="A22" s="5">
         <v>17</v>
       </c>
-      <c r="G6" s="5">
-        <v>1</v>
-      </c>
-      <c r="H6" s="5">
-        <v>3500</v>
-      </c>
-      <c r="I6" s="5"/>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="A7" t="s">
+      <c r="B22" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="G22" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="H22" s="5">
+        <v>1</v>
+      </c>
+      <c r="I22" s="5">
+        <v>14000</v>
+      </c>
+      <c r="J22" s="5"/>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="A23" s="5">
         <v>18</v>
       </c>
-      <c r="B7"/>
-      <c r="C7"/>
-      <c r="D7"/>
-      <c r="E7"/>
-      <c r="F7"/>
-      <c r="G7"/>
-      <c r="H7" t="s">
-        <v>17</v>
-      </c>
-      <c r="I7"/>
-    </row>
-    <row r="8" spans="1:9">
-      <c r="A8" t="s">
+      <c r="B23" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D23" s="5">
+        <v>1</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="H23" s="5">
+        <v>1</v>
+      </c>
+      <c r="I23" s="5">
+        <v>10000</v>
+      </c>
+      <c r="J23" s="5"/>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="A24" s="5">
         <v>19</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B24" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="G24" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="H24" s="5">
+        <v>1</v>
+      </c>
+      <c r="I24" s="5">
+        <v>40000</v>
+      </c>
+      <c r="J24" s="5"/>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="A25" s="5">
         <v>20</v>
       </c>
-      <c r="C8"/>
-      <c r="D8"/>
-      <c r="E8"/>
-      <c r="F8"/>
-      <c r="G8"/>
-      <c r="H8"/>
-    </row>
-    <row r="9" spans="1:9">
-      <c r="A9"/>
-      <c r="B9"/>
-      <c r="C9"/>
-      <c r="D9"/>
-      <c r="E9"/>
-      <c r="F9"/>
-      <c r="G9" t="s">
+      <c r="B25" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="H25" s="5">
+        <v>1</v>
+      </c>
+      <c r="I25" s="5">
+        <v>80000</v>
+      </c>
+      <c r="J25" s="5"/>
+    </row>
+    <row r="26" spans="1:10">
+      <c r="A26" s="5">
         <v>21</v>
       </c>
-      <c r="H9"/>
-    </row>
-    <row r="10" spans="1:9">
-      <c r="A10"/>
-      <c r="B10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C10"/>
-      <c r="D10" t="s">
-        <v>23</v>
-      </c>
-      <c r="E10"/>
-      <c r="F10"/>
-      <c r="G10" t="s">
-        <v>24</v>
-      </c>
-      <c r="H10"/>
-    </row>
-    <row r="14" spans="1:9">
-      <c r="A14"/>
-      <c r="B14"/>
-      <c r="C14"/>
-      <c r="D14"/>
-      <c r="E14"/>
-      <c r="F14"/>
-      <c r="G14"/>
-      <c r="H14"/>
+      <c r="B26" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="G26" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="H26" s="5">
+        <v>1</v>
+      </c>
+      <c r="I26" s="5">
+        <v>80000</v>
+      </c>
+      <c r="J26" s="5"/>
+    </row>
+    <row r="27" spans="1:10">
+      <c r="A27" t="s">
+        <v>66</v>
+      </c>
+      <c r="B27"/>
+      <c r="C27"/>
+      <c r="D27"/>
+      <c r="E27"/>
+      <c r="F27"/>
+      <c r="G27"/>
+      <c r="H27"/>
+      <c r="I27" t="s">
+        <v>67</v>
+      </c>
+      <c r="J27"/>
+    </row>
+    <row r="28" spans="1:10">
+      <c r="A28" t="s">
+        <v>68</v>
+      </c>
+      <c r="B28" t="s">
+        <v>69</v>
+      </c>
+      <c r="C28"/>
+      <c r="D28"/>
+      <c r="E28"/>
+      <c r="F28"/>
+      <c r="G28"/>
+      <c r="H28"/>
+    </row>
+    <row r="29" spans="1:10">
+      <c r="A29"/>
+      <c r="B29"/>
+      <c r="C29"/>
+      <c r="D29"/>
+      <c r="E29"/>
+      <c r="F29"/>
+      <c r="G29" t="s">
+        <v>70</v>
+      </c>
+      <c r="H29"/>
+    </row>
+    <row r="30" spans="1:10">
+      <c r="A30"/>
+      <c r="B30" t="s">
+        <v>71</v>
+      </c>
+      <c r="C30"/>
+      <c r="D30" t="s">
+        <v>72</v>
+      </c>
+      <c r="E30"/>
+      <c r="F30"/>
+      <c r="G30" t="s">
+        <v>73</v>
+      </c>
+      <c r="H30"/>
+    </row>
+    <row r="34" spans="1:10">
+      <c r="A34"/>
+      <c r="B34" t="s">
+        <v>74</v>
+      </c>
+      <c r="C34"/>
+      <c r="D34"/>
+      <c r="E34"/>
+      <c r="F34"/>
+      <c r="G34" t="s">
+        <v>75</v>
+      </c>
+      <c r="H34"/>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>

</xml_diff>